<commit_message>
Sample code: The use of Boolean cell values is somewhat counter intuitive and it is now demonstrated in the most basic sample
</commit_message>
<xml_diff>
--- a/excelExporter/samples/firstSample/EuropeanCapitals.xlsx
+++ b/excelExporter/samples/firstSample/EuropeanCapitals.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32ED0950-F104-4676-BCD5-257F8AECF6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="1320" yWindow="15" windowWidth="27480" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capitals" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
   <si>
     <t>Albania</t>
   </si>
@@ -317,12 +318,15 @@
   </si>
   <si>
     <t>Sarajevo</t>
+  </si>
+  <si>
+    <t>EU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -381,9 +385,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -421,9 +425,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -458,7 +462,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -493,7 +497,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -666,10 +670,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -677,424 +683,580 @@
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>
       <c r="B4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>78</v>
       </c>
       <c r="B8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>88</v>
       </c>
       <c r="B10" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
       <c r="B11" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
       <c r="B13" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
       <c r="B15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
       <c r="B17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>92</v>
       </c>
       <c r="B19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>71</v>
       </c>
       <c r="B20" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>82</v>
       </c>
       <c r="B21" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>94</v>
       </c>
       <c r="B22" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
       <c r="B23" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>84</v>
       </c>
       <c r="B24" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>62</v>
       </c>
       <c r="B26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>75</v>
       </c>
       <c r="B27" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>67</v>
       </c>
       <c r="B29" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
       <c r="B31" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>21</v>
       </c>
       <c r="B32" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>
       <c r="B33" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
       <c r="B34" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>49</v>
       </c>
       <c r="B35" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
       <c r="B36" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
       <c r="B37" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
       <c r="B38" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>56</v>
       </c>
       <c r="B39" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
       <c r="B40" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
       <c r="B41" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>25</v>
       </c>
       <c r="B42" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>31</v>
       </c>
       <c r="B43" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>0</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
       <c r="B45" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>58</v>
       </c>
       <c r="B46" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>96</v>
       </c>
       <c r="B47" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>6</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>53</v>
       </c>
       <c r="B49" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>69</v>
       </c>
       <c r="B50" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>17</v>
       </c>
       <c r="B52" t="s">
         <v>18</v>
       </c>
+      <c r="C52" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B52">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B52">
     <sortCondition ref="B2:B52"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>